<commit_message>
DP ad drop_geo and fix pivot_table geometry bugs
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
+++ b/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
DP create create_age_distribution_table function
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
+++ b/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
@@ -1146,22 +1146,22 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>39951.38161184122</v>
+        <v>-6932.12</v>
       </c>
       <c r="E21" t="n">
         <v>44338</v>
       </c>
       <c r="F21" t="n">
-        <v>9693</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G21" t="n">
         <v>9693</v>
       </c>
       <c r="H21" t="n">
-        <v>-4386.618388158779</v>
+        <v>-51270.12</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>-11233.47111111111</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1182,22 +1182,22 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>30553.66036706011</v>
+        <v>25000</v>
       </c>
       <c r="E22" t="n">
         <v>23884</v>
       </c>
       <c r="F22" t="n">
-        <v>6789.702303791135</v>
+        <v>5555.555555555556</v>
       </c>
       <c r="G22" t="n">
         <v>4110</v>
       </c>
       <c r="H22" t="n">
-        <v>6669.660367060107</v>
+        <v>1116</v>
       </c>
       <c r="I22" t="n">
-        <v>2679.702303791135</v>
+        <v>1445.555555555556</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1218,22 +1218,22 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>29005.76516340315</v>
+        <v>25000</v>
       </c>
       <c r="E23" t="n">
         <v>22674</v>
       </c>
       <c r="F23" t="n">
-        <v>5273.775484255118</v>
+        <v>4545.454545454545</v>
       </c>
       <c r="G23" t="n">
         <v>152</v>
       </c>
       <c r="H23" t="n">
-        <v>6331.765163403154</v>
+        <v>2326</v>
       </c>
       <c r="I23" t="n">
-        <v>5121.775484255118</v>
+        <v>4393.454545454545</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1254,22 +1254,22 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>15440.57446953674</v>
+        <v>25000</v>
       </c>
       <c r="E24" t="n">
         <v>12070</v>
       </c>
       <c r="F24" t="n">
-        <v>2807.377176279408</v>
+        <v>4545.454545454545</v>
       </c>
       <c r="G24" t="n">
         <v>1661</v>
       </c>
       <c r="H24" t="n">
-        <v>3370.574469536741</v>
+        <v>12930</v>
       </c>
       <c r="I24" t="n">
-        <v>1146.377176279408</v>
+        <v>2884.454545454545</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1290,22 +1290,22 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>18151.03593280999</v>
+        <v>-6932.12</v>
       </c>
       <c r="E25" t="n">
         <v>20144</v>
       </c>
       <c r="F25" t="n">
-        <v>4537.758983202499</v>
+        <v>-1733.03</v>
       </c>
       <c r="G25" t="n">
         <v>2618</v>
       </c>
       <c r="H25" t="n">
-        <v>-1992.964067190005</v>
+        <v>-27076.12</v>
       </c>
       <c r="I25" t="n">
-        <v>1919.758983202499</v>
+        <v>-4351.03</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1326,22 +1326,22 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>27115.72301062605</v>
+        <v>-6932.12</v>
       </c>
       <c r="E26" t="n">
         <v>30093</v>
       </c>
       <c r="F26" t="n">
-        <v>6711</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G26" t="n">
         <v>6711</v>
       </c>
       <c r="H26" t="n">
-        <v>-2977.276989373946</v>
+        <v>-37025.12</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>-8251.47111111111</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1644,22 +1644,22 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>17799.62092021091</v>
+        <v>-6932.12</v>
       </c>
       <c r="E35" t="n">
         <v>19754</v>
       </c>
       <c r="F35" t="n">
-        <v>4034</v>
+        <v>-1260.385454545454</v>
       </c>
       <c r="G35" t="n">
         <v>4034</v>
       </c>
       <c r="H35" t="n">
-        <v>-1954.379079789087</v>
+        <v>-26686.12</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>-5294.385454545454</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1680,22 +1680,22 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4380.072759600347</v>
+        <v>-6932.12</v>
       </c>
       <c r="E36" t="n">
         <v>4861</v>
       </c>
       <c r="F36" t="n">
-        <v>1095.018189900087</v>
+        <v>-1733.03</v>
       </c>
       <c r="G36" t="n">
         <v>1449</v>
       </c>
       <c r="H36" t="n">
-        <v>-480.9272403996529</v>
+        <v>-11793.12</v>
       </c>
       <c r="I36" t="n">
-        <v>-353.9818100999132</v>
+        <v>-3182.03</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1716,22 +1716,22 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>13357.37473530458</v>
+        <v>-6932.12</v>
       </c>
       <c r="E37" t="n">
         <v>14824</v>
       </c>
       <c r="F37" t="n">
-        <v>3553</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G37" t="n">
         <v>3553</v>
       </c>
       <c r="H37" t="n">
-        <v>-1466.625264695424</v>
+        <v>-21756.12</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>-5093.471111111111</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -12118,22 +12118,22 @@
         </is>
       </c>
       <c r="D350" t="n">
-        <v>12431.98186879366</v>
+        <v>-6932.12</v>
       </c>
       <c r="E350" t="n">
         <v>13797</v>
       </c>
       <c r="F350" t="n">
-        <v>2762.662637509703</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G350" t="n">
         <v>2225</v>
       </c>
       <c r="H350" t="n">
-        <v>-1365.018131206338</v>
+        <v>-20729.12</v>
       </c>
       <c r="I350" t="n">
-        <v>537.6626375097026</v>
+        <v>-3765.471111111111</v>
       </c>
       <c r="J350" t="inlineStr">
         <is>
@@ -12154,22 +12154,22 @@
         </is>
       </c>
       <c r="D351" t="n">
-        <v>5704.637037858424</v>
+        <v>-6932.12</v>
       </c>
       <c r="E351" t="n">
         <v>6331</v>
       </c>
       <c r="F351" t="n">
-        <v>1166</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G351" t="n">
         <v>1166</v>
       </c>
       <c r="H351" t="n">
-        <v>-626.3629621415757</v>
+        <v>-13263.12</v>
       </c>
       <c r="I351" t="n">
-        <v>0</v>
+        <v>-2706.471111111111</v>
       </c>
       <c r="J351" t="inlineStr">
         <is>
@@ -12190,22 +12190,22 @@
         </is>
       </c>
       <c r="D352" t="n">
-        <v>19691.85560343674</v>
+        <v>-6932.12</v>
       </c>
       <c r="E352" t="n">
         <v>21854</v>
       </c>
       <c r="F352" t="n">
-        <v>4375.967911874831</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G352" t="n">
         <v>3462</v>
       </c>
       <c r="H352" t="n">
-        <v>-2162.144396563261</v>
+        <v>-28786.12</v>
       </c>
       <c r="I352" t="n">
-        <v>913.9679118748309</v>
+        <v>-5002.471111111111</v>
       </c>
       <c r="J352" t="inlineStr">
         <is>
@@ -12258,22 +12258,22 @@
         </is>
       </c>
       <c r="D354" t="n">
-        <v>1950.803851992338</v>
+        <v>-6932.12</v>
       </c>
       <c r="E354" t="n">
         <v>2165</v>
       </c>
       <c r="F354" t="n">
-        <v>433.5119671094083</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G354" t="n">
         <v>647</v>
       </c>
       <c r="H354" t="n">
-        <v>-214.1961480076625</v>
+        <v>-9097.119999999999</v>
       </c>
       <c r="I354" t="n">
-        <v>-213.4880328905917</v>
+        <v>-2187.471111111111</v>
       </c>
       <c r="J354" t="inlineStr">
         <is>
@@ -12294,22 +12294,22 @@
         </is>
       </c>
       <c r="D355" t="n">
-        <v>3489.821394349341</v>
+        <v>-6932.12</v>
       </c>
       <c r="E355" t="n">
         <v>3873</v>
       </c>
       <c r="F355" t="n">
-        <v>775.5158654109646</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G355" t="n">
         <v>1274</v>
       </c>
       <c r="H355" t="n">
-        <v>-383.1786056506594</v>
+        <v>-10805.12</v>
       </c>
       <c r="I355" t="n">
-        <v>-498.4841345890354</v>
+        <v>-2814.471111111111</v>
       </c>
       <c r="J355" t="inlineStr">
         <is>
@@ -12330,22 +12330,22 @@
         </is>
       </c>
       <c r="D356" t="n">
-        <v>17640.13256833902</v>
+        <v>-6932.12</v>
       </c>
       <c r="E356" t="n">
         <v>19577</v>
       </c>
       <c r="F356" t="n">
-        <v>4410.033142084756</v>
+        <v>-1733.03</v>
       </c>
       <c r="G356" t="n">
         <v>3022</v>
       </c>
       <c r="H356" t="n">
-        <v>-1936.867431660976</v>
+        <v>-26509.12</v>
       </c>
       <c r="I356" t="n">
-        <v>1388.033142084756</v>
+        <v>-4755.03</v>
       </c>
       <c r="J356" t="inlineStr">
         <is>
@@ -12366,22 +12366,22 @@
         </is>
       </c>
       <c r="D357" t="n">
-        <v>11256.99423692391</v>
+        <v>-6932.12</v>
       </c>
       <c r="E357" t="n">
         <v>12493</v>
       </c>
       <c r="F357" t="n">
-        <v>2501.55427487198</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G357" t="n">
         <v>993</v>
       </c>
       <c r="H357" t="n">
-        <v>-1236.005763076088</v>
+        <v>-19425.12</v>
       </c>
       <c r="I357" t="n">
-        <v>1508.55427487198</v>
+        <v>-2533.471111111111</v>
       </c>
       <c r="J357" t="inlineStr">
         <is>
@@ -12402,22 +12402,22 @@
         </is>
       </c>
       <c r="D358" t="n">
-        <v>19174.64479002168</v>
+        <v>-6932.12</v>
       </c>
       <c r="E358" t="n">
         <v>21280</v>
       </c>
       <c r="F358" t="n">
-        <v>4671</v>
+        <v>-1733.03</v>
       </c>
       <c r="G358" t="n">
         <v>4671</v>
       </c>
       <c r="H358" t="n">
-        <v>-2105.355209978319</v>
+        <v>-28212.12</v>
       </c>
       <c r="I358" t="n">
-        <v>0</v>
+        <v>-6404.03</v>
       </c>
       <c r="J358" t="inlineStr">
         <is>
@@ -12438,22 +12438,22 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>23556.51967789177</v>
+        <v>-6932.12</v>
       </c>
       <c r="E359" t="n">
         <v>26143</v>
       </c>
       <c r="F359" t="n">
-        <v>4283.003577798503</v>
+        <v>-1260.385454545454</v>
       </c>
       <c r="G359" t="n">
         <v>6099</v>
       </c>
       <c r="H359" t="n">
-        <v>-2586.480322108233</v>
+        <v>-33075.12</v>
       </c>
       <c r="I359" t="n">
-        <v>-1815.996422201497</v>
+        <v>-7359.385454545454</v>
       </c>
       <c r="J359" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
DP fix merge bugs
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
+++ b/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
@@ -1146,22 +1146,22 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>39951.38161184122</v>
+        <v>-6932.12</v>
       </c>
       <c r="E21" t="n">
         <v>44338</v>
       </c>
       <c r="F21" t="n">
-        <v>9693</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G21" t="n">
         <v>9693</v>
       </c>
       <c r="H21" t="n">
-        <v>-4386.618388158779</v>
+        <v>-51270.12</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>-11233.47111111111</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1182,22 +1182,22 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>30553.66036706011</v>
+        <v>25000</v>
       </c>
       <c r="E22" t="n">
         <v>23884</v>
       </c>
       <c r="F22" t="n">
-        <v>6789.702303791135</v>
+        <v>5555.555555555556</v>
       </c>
       <c r="G22" t="n">
         <v>4110</v>
       </c>
       <c r="H22" t="n">
-        <v>6669.660367060107</v>
+        <v>1116</v>
       </c>
       <c r="I22" t="n">
-        <v>2679.702303791135</v>
+        <v>1445.555555555556</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1218,22 +1218,22 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>29005.76516340315</v>
+        <v>25000</v>
       </c>
       <c r="E23" t="n">
         <v>22674</v>
       </c>
       <c r="F23" t="n">
-        <v>5273.775484255118</v>
+        <v>4545.454545454545</v>
       </c>
       <c r="G23" t="n">
         <v>152</v>
       </c>
       <c r="H23" t="n">
-        <v>6331.765163403154</v>
+        <v>2326</v>
       </c>
       <c r="I23" t="n">
-        <v>5121.775484255118</v>
+        <v>4393.454545454545</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1254,22 +1254,22 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>15440.57446953674</v>
+        <v>25000</v>
       </c>
       <c r="E24" t="n">
         <v>12070</v>
       </c>
       <c r="F24" t="n">
-        <v>2807.377176279408</v>
+        <v>4545.454545454545</v>
       </c>
       <c r="G24" t="n">
         <v>1661</v>
       </c>
       <c r="H24" t="n">
-        <v>3370.574469536741</v>
+        <v>12930</v>
       </c>
       <c r="I24" t="n">
-        <v>1146.377176279408</v>
+        <v>2884.454545454545</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1290,22 +1290,22 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>18151.03593280999</v>
+        <v>-6932.12</v>
       </c>
       <c r="E25" t="n">
         <v>20144</v>
       </c>
       <c r="F25" t="n">
-        <v>4537.758983202499</v>
+        <v>-1733.03</v>
       </c>
       <c r="G25" t="n">
         <v>2618</v>
       </c>
       <c r="H25" t="n">
-        <v>-1992.964067190005</v>
+        <v>-27076.12</v>
       </c>
       <c r="I25" t="n">
-        <v>1919.758983202499</v>
+        <v>-4351.03</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1326,22 +1326,22 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>27115.72301062605</v>
+        <v>-6932.12</v>
       </c>
       <c r="E26" t="n">
         <v>30093</v>
       </c>
       <c r="F26" t="n">
-        <v>6711</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G26" t="n">
         <v>6711</v>
       </c>
       <c r="H26" t="n">
-        <v>-2977.276989373946</v>
+        <v>-37025.12</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>-8251.47111111111</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1644,22 +1644,22 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>17799.62092021091</v>
+        <v>-6932.12</v>
       </c>
       <c r="E35" t="n">
         <v>19754</v>
       </c>
       <c r="F35" t="n">
-        <v>4034</v>
+        <v>-1260.385454545454</v>
       </c>
       <c r="G35" t="n">
         <v>4034</v>
       </c>
       <c r="H35" t="n">
-        <v>-1954.379079789087</v>
+        <v>-26686.12</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>-5294.385454545454</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1680,22 +1680,22 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4380.072759600347</v>
+        <v>-6932.12</v>
       </c>
       <c r="E36" t="n">
         <v>4861</v>
       </c>
       <c r="F36" t="n">
-        <v>1095.018189900087</v>
+        <v>-1733.03</v>
       </c>
       <c r="G36" t="n">
         <v>1449</v>
       </c>
       <c r="H36" t="n">
-        <v>-480.9272403996529</v>
+        <v>-11793.12</v>
       </c>
       <c r="I36" t="n">
-        <v>-353.9818100999132</v>
+        <v>-3182.03</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1716,22 +1716,22 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>13357.37473530458</v>
+        <v>-6932.12</v>
       </c>
       <c r="E37" t="n">
         <v>14824</v>
       </c>
       <c r="F37" t="n">
-        <v>3553</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G37" t="n">
         <v>3553</v>
       </c>
       <c r="H37" t="n">
-        <v>-1466.625264695424</v>
+        <v>-21756.12</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>-5093.471111111111</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -12118,22 +12118,22 @@
         </is>
       </c>
       <c r="D350" t="n">
-        <v>12431.98186879366</v>
+        <v>-6932.12</v>
       </c>
       <c r="E350" t="n">
         <v>13797</v>
       </c>
       <c r="F350" t="n">
-        <v>2762.662637509703</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G350" t="n">
         <v>2225</v>
       </c>
       <c r="H350" t="n">
-        <v>-1365.018131206338</v>
+        <v>-20729.12</v>
       </c>
       <c r="I350" t="n">
-        <v>537.6626375097026</v>
+        <v>-3765.471111111111</v>
       </c>
       <c r="J350" t="inlineStr">
         <is>
@@ -12154,22 +12154,22 @@
         </is>
       </c>
       <c r="D351" t="n">
-        <v>5704.637037858424</v>
+        <v>-6932.12</v>
       </c>
       <c r="E351" t="n">
         <v>6331</v>
       </c>
       <c r="F351" t="n">
-        <v>1166</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G351" t="n">
         <v>1166</v>
       </c>
       <c r="H351" t="n">
-        <v>-626.3629621415757</v>
+        <v>-13263.12</v>
       </c>
       <c r="I351" t="n">
-        <v>0</v>
+        <v>-2706.471111111111</v>
       </c>
       <c r="J351" t="inlineStr">
         <is>
@@ -12190,22 +12190,22 @@
         </is>
       </c>
       <c r="D352" t="n">
-        <v>19691.85560343674</v>
+        <v>-6932.12</v>
       </c>
       <c r="E352" t="n">
         <v>21854</v>
       </c>
       <c r="F352" t="n">
-        <v>4375.967911874831</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G352" t="n">
         <v>3462</v>
       </c>
       <c r="H352" t="n">
-        <v>-2162.144396563261</v>
+        <v>-28786.12</v>
       </c>
       <c r="I352" t="n">
-        <v>913.9679118748309</v>
+        <v>-5002.471111111111</v>
       </c>
       <c r="J352" t="inlineStr">
         <is>
@@ -12258,22 +12258,22 @@
         </is>
       </c>
       <c r="D354" t="n">
-        <v>1950.803851992338</v>
+        <v>-6932.12</v>
       </c>
       <c r="E354" t="n">
         <v>2165</v>
       </c>
       <c r="F354" t="n">
-        <v>433.5119671094083</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G354" t="n">
         <v>647</v>
       </c>
       <c r="H354" t="n">
-        <v>-214.1961480076625</v>
+        <v>-9097.119999999999</v>
       </c>
       <c r="I354" t="n">
-        <v>-213.4880328905917</v>
+        <v>-2187.471111111111</v>
       </c>
       <c r="J354" t="inlineStr">
         <is>
@@ -12294,22 +12294,22 @@
         </is>
       </c>
       <c r="D355" t="n">
-        <v>3489.821394349341</v>
+        <v>-6932.12</v>
       </c>
       <c r="E355" t="n">
         <v>3873</v>
       </c>
       <c r="F355" t="n">
-        <v>775.5158654109646</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G355" t="n">
         <v>1274</v>
       </c>
       <c r="H355" t="n">
-        <v>-383.1786056506594</v>
+        <v>-10805.12</v>
       </c>
       <c r="I355" t="n">
-        <v>-498.4841345890354</v>
+        <v>-2814.471111111111</v>
       </c>
       <c r="J355" t="inlineStr">
         <is>
@@ -12330,22 +12330,22 @@
         </is>
       </c>
       <c r="D356" t="n">
-        <v>17640.13256833902</v>
+        <v>-6932.12</v>
       </c>
       <c r="E356" t="n">
         <v>19577</v>
       </c>
       <c r="F356" t="n">
-        <v>4410.033142084756</v>
+        <v>-1733.03</v>
       </c>
       <c r="G356" t="n">
         <v>3022</v>
       </c>
       <c r="H356" t="n">
-        <v>-1936.867431660976</v>
+        <v>-26509.12</v>
       </c>
       <c r="I356" t="n">
-        <v>1388.033142084756</v>
+        <v>-4755.03</v>
       </c>
       <c r="J356" t="inlineStr">
         <is>
@@ -12366,22 +12366,22 @@
         </is>
       </c>
       <c r="D357" t="n">
-        <v>11256.99423692391</v>
+        <v>-6932.12</v>
       </c>
       <c r="E357" t="n">
         <v>12493</v>
       </c>
       <c r="F357" t="n">
-        <v>2501.55427487198</v>
+        <v>-1540.471111111111</v>
       </c>
       <c r="G357" t="n">
         <v>993</v>
       </c>
       <c r="H357" t="n">
-        <v>-1236.005763076088</v>
+        <v>-19425.12</v>
       </c>
       <c r="I357" t="n">
-        <v>1508.55427487198</v>
+        <v>-2533.471111111111</v>
       </c>
       <c r="J357" t="inlineStr">
         <is>
@@ -12402,22 +12402,22 @@
         </is>
       </c>
       <c r="D358" t="n">
-        <v>19174.64479002168</v>
+        <v>-6932.12</v>
       </c>
       <c r="E358" t="n">
         <v>21280</v>
       </c>
       <c r="F358" t="n">
-        <v>4671</v>
+        <v>-1733.03</v>
       </c>
       <c r="G358" t="n">
         <v>4671</v>
       </c>
       <c r="H358" t="n">
-        <v>-2105.355209978319</v>
+        <v>-28212.12</v>
       </c>
       <c r="I358" t="n">
-        <v>0</v>
+        <v>-6404.03</v>
       </c>
       <c r="J358" t="inlineStr">
         <is>
@@ -12438,22 +12438,22 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>23556.51967789177</v>
+        <v>-6932.12</v>
       </c>
       <c r="E359" t="n">
         <v>26143</v>
       </c>
       <c r="F359" t="n">
-        <v>4283.003577798503</v>
+        <v>-1260.385454545454</v>
       </c>
       <c r="G359" t="n">
         <v>6099</v>
       </c>
       <c r="H359" t="n">
-        <v>-2586.480322108233</v>
+        <v>-33075.12</v>
       </c>
       <c r="I359" t="n">
-        <v>-1815.996422201497</v>
+        <v>-7359.385454545454</v>
       </c>
       <c r="J359" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
DP: Resetting the code to the initial - Fix the geometry pivot bug - fix_cbs_data_230717
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
+++ b/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
DP: main - cleanup after merge
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
+++ b/create_forecast_basic/current/Intermediates/stat_cbs_jtmt_2020_short.xlsx
@@ -1146,22 +1146,22 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>-6932.12</v>
+        <v>39951.38161184122</v>
       </c>
       <c r="E21" t="n">
         <v>44338</v>
       </c>
       <c r="F21" t="n">
-        <v>-1540.471111111111</v>
+        <v>9693</v>
       </c>
       <c r="G21" t="n">
         <v>9693</v>
       </c>
       <c r="H21" t="n">
-        <v>-51270.12</v>
+        <v>-4386.618388158779</v>
       </c>
       <c r="I21" t="n">
-        <v>-11233.47111111111</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1182,22 +1182,22 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>25000</v>
+        <v>30553.66036706011</v>
       </c>
       <c r="E22" t="n">
         <v>23884</v>
       </c>
       <c r="F22" t="n">
-        <v>5555.555555555556</v>
+        <v>6789.702303791135</v>
       </c>
       <c r="G22" t="n">
         <v>4110</v>
       </c>
       <c r="H22" t="n">
-        <v>1116</v>
+        <v>6669.660367060107</v>
       </c>
       <c r="I22" t="n">
-        <v>1445.555555555556</v>
+        <v>2679.702303791135</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1218,22 +1218,22 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>25000</v>
+        <v>29005.76516340315</v>
       </c>
       <c r="E23" t="n">
         <v>22674</v>
       </c>
       <c r="F23" t="n">
-        <v>4545.454545454545</v>
+        <v>5273.775484255118</v>
       </c>
       <c r="G23" t="n">
         <v>152</v>
       </c>
       <c r="H23" t="n">
-        <v>2326</v>
+        <v>6331.765163403154</v>
       </c>
       <c r="I23" t="n">
-        <v>4393.454545454545</v>
+        <v>5121.775484255118</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1254,22 +1254,22 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>25000</v>
+        <v>15440.57446953674</v>
       </c>
       <c r="E24" t="n">
         <v>12070</v>
       </c>
       <c r="F24" t="n">
-        <v>4545.454545454545</v>
+        <v>2807.377176279408</v>
       </c>
       <c r="G24" t="n">
         <v>1661</v>
       </c>
       <c r="H24" t="n">
-        <v>12930</v>
+        <v>3370.574469536741</v>
       </c>
       <c r="I24" t="n">
-        <v>2884.454545454545</v>
+        <v>1146.377176279408</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1290,22 +1290,22 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>-6932.12</v>
+        <v>18151.03593280999</v>
       </c>
       <c r="E25" t="n">
         <v>20144</v>
       </c>
       <c r="F25" t="n">
-        <v>-1733.03</v>
+        <v>4537.758983202499</v>
       </c>
       <c r="G25" t="n">
         <v>2618</v>
       </c>
       <c r="H25" t="n">
-        <v>-27076.12</v>
+        <v>-1992.964067190005</v>
       </c>
       <c r="I25" t="n">
-        <v>-4351.03</v>
+        <v>1919.758983202499</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1326,22 +1326,22 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>-6932.12</v>
+        <v>27115.72301062605</v>
       </c>
       <c r="E26" t="n">
         <v>30093</v>
       </c>
       <c r="F26" t="n">
-        <v>-1540.471111111111</v>
+        <v>6711</v>
       </c>
       <c r="G26" t="n">
         <v>6711</v>
       </c>
       <c r="H26" t="n">
-        <v>-37025.12</v>
+        <v>-2977.276989373946</v>
       </c>
       <c r="I26" t="n">
-        <v>-8251.47111111111</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1644,22 +1644,22 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>-6932.12</v>
+        <v>17799.62092021091</v>
       </c>
       <c r="E35" t="n">
         <v>19754</v>
       </c>
       <c r="F35" t="n">
-        <v>-1260.385454545454</v>
+        <v>4034</v>
       </c>
       <c r="G35" t="n">
         <v>4034</v>
       </c>
       <c r="H35" t="n">
-        <v>-26686.12</v>
+        <v>-1954.379079789087</v>
       </c>
       <c r="I35" t="n">
-        <v>-5294.385454545454</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1680,22 +1680,22 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>-6932.12</v>
+        <v>4380.072759600347</v>
       </c>
       <c r="E36" t="n">
         <v>4861</v>
       </c>
       <c r="F36" t="n">
-        <v>-1733.03</v>
+        <v>1095.018189900087</v>
       </c>
       <c r="G36" t="n">
         <v>1449</v>
       </c>
       <c r="H36" t="n">
-        <v>-11793.12</v>
+        <v>-480.9272403996529</v>
       </c>
       <c r="I36" t="n">
-        <v>-3182.03</v>
+        <v>-353.9818100999132</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1716,22 +1716,22 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>-6932.12</v>
+        <v>13357.37473530458</v>
       </c>
       <c r="E37" t="n">
         <v>14824</v>
       </c>
       <c r="F37" t="n">
-        <v>-1540.471111111111</v>
+        <v>3553</v>
       </c>
       <c r="G37" t="n">
         <v>3553</v>
       </c>
       <c r="H37" t="n">
-        <v>-21756.12</v>
+        <v>-1466.625264695424</v>
       </c>
       <c r="I37" t="n">
-        <v>-5093.471111111111</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -12118,22 +12118,22 @@
         </is>
       </c>
       <c r="D350" t="n">
-        <v>-6932.12</v>
+        <v>12431.98186879366</v>
       </c>
       <c r="E350" t="n">
         <v>13797</v>
       </c>
       <c r="F350" t="n">
-        <v>-1540.471111111111</v>
+        <v>2762.662637509703</v>
       </c>
       <c r="G350" t="n">
         <v>2225</v>
       </c>
       <c r="H350" t="n">
-        <v>-20729.12</v>
+        <v>-1365.018131206338</v>
       </c>
       <c r="I350" t="n">
-        <v>-3765.471111111111</v>
+        <v>537.6626375097026</v>
       </c>
       <c r="J350" t="inlineStr">
         <is>
@@ -12154,22 +12154,22 @@
         </is>
       </c>
       <c r="D351" t="n">
-        <v>-6932.12</v>
+        <v>5704.637037858424</v>
       </c>
       <c r="E351" t="n">
         <v>6331</v>
       </c>
       <c r="F351" t="n">
-        <v>-1540.471111111111</v>
+        <v>1166</v>
       </c>
       <c r="G351" t="n">
         <v>1166</v>
       </c>
       <c r="H351" t="n">
-        <v>-13263.12</v>
+        <v>-626.3629621415757</v>
       </c>
       <c r="I351" t="n">
-        <v>-2706.471111111111</v>
+        <v>0</v>
       </c>
       <c r="J351" t="inlineStr">
         <is>
@@ -12190,22 +12190,22 @@
         </is>
       </c>
       <c r="D352" t="n">
-        <v>-6932.12</v>
+        <v>19691.85560343674</v>
       </c>
       <c r="E352" t="n">
         <v>21854</v>
       </c>
       <c r="F352" t="n">
-        <v>-1540.471111111111</v>
+        <v>4375.967911874831</v>
       </c>
       <c r="G352" t="n">
         <v>3462</v>
       </c>
       <c r="H352" t="n">
-        <v>-28786.12</v>
+        <v>-2162.144396563261</v>
       </c>
       <c r="I352" t="n">
-        <v>-5002.471111111111</v>
+        <v>913.9679118748309</v>
       </c>
       <c r="J352" t="inlineStr">
         <is>
@@ -12258,22 +12258,22 @@
         </is>
       </c>
       <c r="D354" t="n">
-        <v>-6932.12</v>
+        <v>1950.803851992338</v>
       </c>
       <c r="E354" t="n">
         <v>2165</v>
       </c>
       <c r="F354" t="n">
-        <v>-1540.471111111111</v>
+        <v>433.5119671094083</v>
       </c>
       <c r="G354" t="n">
         <v>647</v>
       </c>
       <c r="H354" t="n">
-        <v>-9097.119999999999</v>
+        <v>-214.1961480076625</v>
       </c>
       <c r="I354" t="n">
-        <v>-2187.471111111111</v>
+        <v>-213.4880328905917</v>
       </c>
       <c r="J354" t="inlineStr">
         <is>
@@ -12294,22 +12294,22 @@
         </is>
       </c>
       <c r="D355" t="n">
-        <v>-6932.12</v>
+        <v>3489.821394349341</v>
       </c>
       <c r="E355" t="n">
         <v>3873</v>
       </c>
       <c r="F355" t="n">
-        <v>-1540.471111111111</v>
+        <v>775.5158654109646</v>
       </c>
       <c r="G355" t="n">
         <v>1274</v>
       </c>
       <c r="H355" t="n">
-        <v>-10805.12</v>
+        <v>-383.1786056506594</v>
       </c>
       <c r="I355" t="n">
-        <v>-2814.471111111111</v>
+        <v>-498.4841345890354</v>
       </c>
       <c r="J355" t="inlineStr">
         <is>
@@ -12330,22 +12330,22 @@
         </is>
       </c>
       <c r="D356" t="n">
-        <v>-6932.12</v>
+        <v>17640.13256833902</v>
       </c>
       <c r="E356" t="n">
         <v>19577</v>
       </c>
       <c r="F356" t="n">
-        <v>-1733.03</v>
+        <v>4410.033142084756</v>
       </c>
       <c r="G356" t="n">
         <v>3022</v>
       </c>
       <c r="H356" t="n">
-        <v>-26509.12</v>
+        <v>-1936.867431660976</v>
       </c>
       <c r="I356" t="n">
-        <v>-4755.03</v>
+        <v>1388.033142084756</v>
       </c>
       <c r="J356" t="inlineStr">
         <is>
@@ -12366,22 +12366,22 @@
         </is>
       </c>
       <c r="D357" t="n">
-        <v>-6932.12</v>
+        <v>11256.99423692391</v>
       </c>
       <c r="E357" t="n">
         <v>12493</v>
       </c>
       <c r="F357" t="n">
-        <v>-1540.471111111111</v>
+        <v>2501.55427487198</v>
       </c>
       <c r="G357" t="n">
         <v>993</v>
       </c>
       <c r="H357" t="n">
-        <v>-19425.12</v>
+        <v>-1236.005763076088</v>
       </c>
       <c r="I357" t="n">
-        <v>-2533.471111111111</v>
+        <v>1508.55427487198</v>
       </c>
       <c r="J357" t="inlineStr">
         <is>
@@ -12402,22 +12402,22 @@
         </is>
       </c>
       <c r="D358" t="n">
-        <v>-6932.12</v>
+        <v>19174.64479002168</v>
       </c>
       <c r="E358" t="n">
         <v>21280</v>
       </c>
       <c r="F358" t="n">
-        <v>-1733.03</v>
+        <v>4671</v>
       </c>
       <c r="G358" t="n">
         <v>4671</v>
       </c>
       <c r="H358" t="n">
-        <v>-28212.12</v>
+        <v>-2105.355209978319</v>
       </c>
       <c r="I358" t="n">
-        <v>-6404.03</v>
+        <v>0</v>
       </c>
       <c r="J358" t="inlineStr">
         <is>
@@ -12438,22 +12438,22 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>-6932.12</v>
+        <v>23556.51967789177</v>
       </c>
       <c r="E359" t="n">
         <v>26143</v>
       </c>
       <c r="F359" t="n">
-        <v>-1260.385454545454</v>
+        <v>4283.003577798503</v>
       </c>
       <c r="G359" t="n">
         <v>6099</v>
       </c>
       <c r="H359" t="n">
-        <v>-33075.12</v>
+        <v>-2586.480322108233</v>
       </c>
       <c r="I359" t="n">
-        <v>-7359.385454545454</v>
+        <v>-1815.996422201497</v>
       </c>
       <c r="J359" t="inlineStr">
         <is>

</xml_diff>